<commit_message>
version 6 - Clase nombreServicio
Se agrega la clase nombreServicio con su .h de funciones. Se reforma movimientoServicios y se corrigen y optimizan funciones.
</commit_message>
<xml_diff>
--- a/Dataset inicial.xlsx
+++ b/Dataset inicial.xlsx
@@ -4,28 +4,30 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="30" windowWidth="18915" windowHeight="7755" activeTab="3"/>
+    <workbookView xWindow="480" yWindow="30" windowWidth="18915" windowHeight="7755" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="MOVIMIENTOS" sheetId="2" r:id="rId1"/>
     <sheet name="MOVIMIENTOS REDUCIDA" sheetId="5" r:id="rId2"/>
     <sheet name="MOVIMIENTO SERVICIO" sheetId="3" r:id="rId3"/>
-    <sheet name="NOMBRES SERVICIOS" sheetId="7" r:id="rId4"/>
-    <sheet name="CATEGORIAS" sheetId="1" r:id="rId5"/>
-    <sheet name="AHORRO" sheetId="4" r:id="rId6"/>
+    <sheet name="MOVIMIENTO SERVICIO (2)" sheetId="8" r:id="rId4"/>
+    <sheet name="NOMBRES SERVICIOS" sheetId="7" r:id="rId5"/>
+    <sheet name="CATEGORIAS" sheetId="1" r:id="rId6"/>
+    <sheet name="AHORRO" sheetId="4" r:id="rId7"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'MOVIMIENTO SERVICIO'!$C$2:$C$20</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'MOVIMIENTO SERVICIO (2)'!$C$2:$C$20</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">MOVIMIENTOS!$B$2:$H$83</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'MOVIMIENTOS REDUCIDA'!$B$2:$H$60</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">'NOMBRES SERVICIOS'!$C$2:$C$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'NOMBRES SERVICIOS'!$C$2:$C$11</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="53">
   <si>
     <t>TIPO MOVIMIENTO</t>
   </si>
@@ -177,6 +179,15 @@
   </si>
   <si>
     <t>N</t>
+  </si>
+  <si>
+    <t>NOMBRES SERVICIOS</t>
+  </si>
+  <si>
+    <t>COD NOMBRE</t>
+  </si>
+  <si>
+    <t>MOVIMIENTO SERVICIO</t>
   </si>
 </sst>
 </file>
@@ -1068,11 +1079,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
-  <dimension ref="B3:L84"/>
+  <dimension ref="B2:L83"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1087,7 +1097,8 @@
     <col min="11" max="11" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:11" ht="16.5" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:11" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="35" t="s">
         <v>24</v>
       </c>
@@ -1110,7 +1121,7 @@
       </c>
       <c r="K3" s="34"/>
     </row>
-    <row r="4" spans="2:11" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="36"/>
       <c r="C4" s="7" t="s">
         <v>43</v>
@@ -1131,7 +1142,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="2:11" ht="16.5" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="2:11" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="31">
         <v>1</v>
       </c>
@@ -1158,7 +1169,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B6" s="32">
         <v>2</v>
       </c>
@@ -1260,7 +1271,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="10" spans="2:11" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B10" s="32">
         <v>6</v>
       </c>
@@ -1289,7 +1300,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="2:11" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:11" x14ac:dyDescent="0.25">
       <c r="B11" s="32">
         <v>7</v>
       </c>
@@ -1312,7 +1323,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="32">
         <v>8</v>
       </c>
@@ -1335,7 +1346,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="32">
         <v>9</v>
       </c>
@@ -1360,7 +1371,7 @@
       </c>
       <c r="K13" s="34"/>
     </row>
-    <row r="14" spans="2:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="32">
         <v>10</v>
       </c>
@@ -1387,7 +1398,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="32">
         <v>11</v>
       </c>
@@ -1511,7 +1522,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="32">
         <v>16</v>
       </c>
@@ -1534,7 +1545,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="32">
         <v>17</v>
       </c>
@@ -1557,7 +1568,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="22" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="32">
         <v>18</v>
       </c>
@@ -1580,7 +1591,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="23" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="32">
         <v>19</v>
       </c>
@@ -1601,7 +1612,7 @@
       </c>
       <c r="H23" s="6"/>
     </row>
-    <row r="24" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="32">
         <v>20</v>
       </c>
@@ -1624,7 +1635,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="32">
         <v>21</v>
       </c>
@@ -1647,7 +1658,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="32">
         <v>22</v>
       </c>
@@ -1716,7 +1727,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="32">
         <v>25</v>
       </c>
@@ -1739,7 +1750,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="30" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="32">
         <v>26</v>
       </c>
@@ -1760,7 +1771,7 @@
       </c>
       <c r="H30" s="6"/>
     </row>
-    <row r="31" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="32">
         <v>27</v>
       </c>
@@ -1781,7 +1792,7 @@
       </c>
       <c r="H31" s="6"/>
     </row>
-    <row r="32" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="32">
         <v>28</v>
       </c>
@@ -1802,7 +1813,7 @@
       </c>
       <c r="H32" s="6"/>
     </row>
-    <row r="33" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="32">
         <v>29</v>
       </c>
@@ -1825,7 +1836,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="34" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="32">
         <v>30</v>
       </c>
@@ -1848,7 +1859,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="32">
         <v>31</v>
       </c>
@@ -1894,7 +1905,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="32">
         <v>33</v>
       </c>
@@ -1915,7 +1926,7 @@
       </c>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="32">
         <v>34</v>
       </c>
@@ -1936,7 +1947,7 @@
       </c>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="32">
         <v>35</v>
       </c>
@@ -1957,7 +1968,7 @@
       </c>
       <c r="H39" s="6"/>
     </row>
-    <row r="40" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="32">
         <v>36</v>
       </c>
@@ -2003,7 +2014,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="42" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="32">
         <v>38</v>
       </c>
@@ -2026,7 +2037,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="43" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="32">
         <v>39</v>
       </c>
@@ -2072,7 +2083,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="32">
         <v>41</v>
       </c>
@@ -2093,7 +2104,7 @@
       </c>
       <c r="H45" s="6"/>
     </row>
-    <row r="46" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="32">
         <v>42</v>
       </c>
@@ -2114,7 +2125,7 @@
       </c>
       <c r="H46" s="6"/>
     </row>
-    <row r="47" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="32">
         <v>43</v>
       </c>
@@ -2137,7 +2148,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="32">
         <v>44</v>
       </c>
@@ -2160,7 +2171,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="49" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="32">
         <v>45</v>
       </c>
@@ -2229,7 +2240,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="32">
         <v>48</v>
       </c>
@@ -2250,7 +2261,7 @@
       </c>
       <c r="H52" s="6"/>
     </row>
-    <row r="53" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B53" s="32">
         <v>49</v>
       </c>
@@ -2273,7 +2284,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="54" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B54" s="32">
         <v>50</v>
       </c>
@@ -2296,7 +2307,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="55" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B55" s="32">
         <v>51</v>
       </c>
@@ -2319,7 +2330,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="56" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B56" s="32">
         <v>52</v>
       </c>
@@ -2388,7 +2399,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B59" s="32">
         <v>55</v>
       </c>
@@ -2409,7 +2420,7 @@
       </c>
       <c r="H59" s="6"/>
     </row>
-    <row r="60" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B60" s="32">
         <v>56</v>
       </c>
@@ -2430,7 +2441,7 @@
       </c>
       <c r="H60" s="6"/>
     </row>
-    <row r="61" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B61" s="32">
         <v>57</v>
       </c>
@@ -2453,7 +2464,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="62" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B62" s="32">
         <v>58</v>
       </c>
@@ -2545,7 +2556,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="66" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B66" s="32">
         <v>62</v>
       </c>
@@ -2566,7 +2577,7 @@
       </c>
       <c r="H66" s="6"/>
     </row>
-    <row r="67" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B67" s="32">
         <v>63</v>
       </c>
@@ -2587,7 +2598,7 @@
       </c>
       <c r="H67" s="6"/>
     </row>
-    <row r="68" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B68" s="32">
         <v>64</v>
       </c>
@@ -2608,7 +2619,7 @@
       </c>
       <c r="H68" s="6"/>
     </row>
-    <row r="69" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B69" s="32">
         <v>65</v>
       </c>
@@ -2631,7 +2642,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="70" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B70" s="32">
         <v>66</v>
       </c>
@@ -2654,7 +2665,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="71" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B71" s="32">
         <v>67</v>
       </c>
@@ -2677,7 +2688,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="72" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B72" s="32">
         <v>68</v>
       </c>
@@ -2698,7 +2709,7 @@
       </c>
       <c r="H72" s="6"/>
     </row>
-    <row r="73" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B73" s="32">
         <v>69</v>
       </c>
@@ -2721,7 +2732,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="74" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B74" s="32">
         <v>70</v>
       </c>
@@ -2790,7 +2801,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="77" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B77" s="32">
         <v>73</v>
       </c>
@@ -2811,7 +2822,7 @@
       </c>
       <c r="H77" s="6"/>
     </row>
-    <row r="78" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B78" s="32">
         <v>74</v>
       </c>
@@ -2832,7 +2843,7 @@
       </c>
       <c r="H78" s="6"/>
     </row>
-    <row r="79" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B79" s="32">
         <v>75</v>
       </c>
@@ -2855,7 +2866,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="80" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B80" s="32">
         <v>76</v>
       </c>
@@ -2901,8 +2912,8 @@
         <v>48</v>
       </c>
     </row>
-    <row r="82" spans="2:11" ht="15.75" hidden="1" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="83" spans="2:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="83" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F83" s="1"/>
       <c r="G83" s="1"/>
       <c r="H83" s="1"/>
@@ -2910,15 +2921,8 @@
       <c r="J83" s="1"/>
       <c r="K83" s="1"/>
     </row>
-    <row r="84" spans="2:11" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <autoFilter ref="B2:H83">
-    <filterColumn colId="5">
-      <filters>
-        <filter val="7"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B2:H83"/>
   <mergeCells count="8">
     <mergeCell ref="J3:K3"/>
     <mergeCell ref="B3:B4"/>
@@ -2936,11 +2940,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <sheetPr filterMode="1"/>
   <dimension ref="B2:L83"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G58" sqref="G58"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2956,7 +2959,7 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="3" spans="2:11" ht="16.5" hidden="1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="2:11" ht="16.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B3" s="35" t="s">
         <v>24</v>
       </c>
@@ -2979,7 +2982,7 @@
       </c>
       <c r="K3" s="34"/>
     </row>
-    <row r="4" spans="2:11" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="36"/>
       <c r="C4" s="7" t="s">
         <v>43</v>
@@ -3177,7 +3180,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="12" spans="2:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B12" s="32">
         <v>8</v>
       </c>
@@ -3200,7 +3203,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="2:11" ht="15.75" hidden="1" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B13" s="32">
         <v>15</v>
       </c>
@@ -3225,7 +3228,7 @@
       </c>
       <c r="K13" s="44"/>
     </row>
-    <row r="14" spans="2:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="32">
         <v>16</v>
       </c>
@@ -3254,7 +3257,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="15" spans="2:11" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="32">
         <v>20</v>
       </c>
@@ -3283,7 +3286,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="16" spans="2:11" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="32">
         <v>21</v>
       </c>
@@ -3306,7 +3309,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="17" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="32">
         <v>22</v>
       </c>
@@ -3327,7 +3330,7 @@
       </c>
       <c r="H17" s="6"/>
     </row>
-    <row r="18" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="32">
         <v>23</v>
       </c>
@@ -3348,7 +3351,7 @@
       </c>
       <c r="H18" s="6"/>
     </row>
-    <row r="19" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="32">
         <v>24</v>
       </c>
@@ -3374,7 +3377,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="32">
         <v>25</v>
       </c>
@@ -3397,7 +3400,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="21" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="32">
         <v>26</v>
       </c>
@@ -3418,7 +3421,7 @@
       </c>
       <c r="H21" s="6"/>
     </row>
-    <row r="22" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="32">
         <v>27</v>
       </c>
@@ -3439,7 +3442,7 @@
       </c>
       <c r="H22" s="6"/>
     </row>
-    <row r="23" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B23" s="32">
         <v>28</v>
       </c>
@@ -3462,7 +3465,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="24" spans="2:12" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B24" s="32">
         <v>29</v>
       </c>
@@ -3485,7 +3488,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="25" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="32">
         <v>30</v>
       </c>
@@ -3506,7 +3509,7 @@
       </c>
       <c r="H25" s="6"/>
     </row>
-    <row r="26" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B26" s="32">
         <v>31</v>
       </c>
@@ -3527,7 +3530,7 @@
       </c>
       <c r="H26" s="6"/>
     </row>
-    <row r="27" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="32">
         <v>32</v>
       </c>
@@ -3550,7 +3553,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="28" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="32">
         <v>33</v>
       </c>
@@ -3573,7 +3576,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="29" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="32">
         <v>34</v>
       </c>
@@ -3594,7 +3597,7 @@
       </c>
       <c r="H29" s="6"/>
     </row>
-    <row r="30" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="32">
         <v>35</v>
       </c>
@@ -3617,7 +3620,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="31" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B31" s="32">
         <v>36</v>
       </c>
@@ -3640,7 +3643,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="32" spans="2:12" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B32" s="32">
         <v>37</v>
       </c>
@@ -3663,7 +3666,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="33" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B33" s="32">
         <v>38</v>
       </c>
@@ -3684,7 +3687,7 @@
       </c>
       <c r="H33" s="6"/>
     </row>
-    <row r="34" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B34" s="32">
         <v>39</v>
       </c>
@@ -3707,7 +3710,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="35" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B35" s="32">
         <v>40</v>
       </c>
@@ -3730,7 +3733,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="36" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B36" s="32">
         <v>41</v>
       </c>
@@ -3753,7 +3756,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="37" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="32">
         <v>42</v>
       </c>
@@ -3774,7 +3777,7 @@
       </c>
       <c r="H37" s="6"/>
     </row>
-    <row r="38" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B38" s="32">
         <v>43</v>
       </c>
@@ -3795,7 +3798,7 @@
       </c>
       <c r="H38" s="6"/>
     </row>
-    <row r="39" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B39" s="32">
         <v>44</v>
       </c>
@@ -3818,7 +3821,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="40" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B40" s="32">
         <v>45</v>
       </c>
@@ -3841,7 +3844,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="41" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B41" s="32">
         <v>46</v>
       </c>
@@ -3862,7 +3865,7 @@
       </c>
       <c r="H41" s="6"/>
     </row>
-    <row r="42" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B42" s="32">
         <v>47</v>
       </c>
@@ -3885,7 +3888,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="43" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B43" s="32">
         <v>48</v>
       </c>
@@ -3908,7 +3911,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="44" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B44" s="32">
         <v>49</v>
       </c>
@@ -3931,7 +3934,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="32">
         <v>50</v>
       </c>
@@ -3952,7 +3955,7 @@
       </c>
       <c r="H45" s="6"/>
     </row>
-    <row r="46" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B46" s="32">
         <v>51</v>
       </c>
@@ -3973,7 +3976,7 @@
       </c>
       <c r="H46" s="6"/>
     </row>
-    <row r="47" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B47" s="32">
         <v>52</v>
       </c>
@@ -3996,7 +3999,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="48" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B48" s="32">
         <v>53</v>
       </c>
@@ -4019,7 +4022,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B49" s="32">
         <v>54</v>
       </c>
@@ -4040,7 +4043,7 @@
       </c>
       <c r="H49" s="6"/>
     </row>
-    <row r="50" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B50" s="32">
         <v>55</v>
       </c>
@@ -4063,7 +4066,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="51" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B51" s="32">
         <v>56</v>
       </c>
@@ -4086,7 +4089,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="52" spans="2:8" ht="15" hidden="1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B52" s="32">
         <v>57</v>
       </c>
@@ -4307,14 +4310,7 @@
       <c r="K83" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:H60">
-    <filterColumn colId="2">
-      <filters>
-        <filter val="5"/>
-        <filter val="6"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
+  <autoFilter ref="B2:H60"/>
   <mergeCells count="8">
     <mergeCell ref="J8:K8"/>
     <mergeCell ref="J13:K13"/>
@@ -4335,7 +4331,7 @@
   <dimension ref="B2:I20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C3" sqref="C3:C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4688,10 +4684,371 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:C12"/>
+  <dimension ref="B2:I22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3:C11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="5.140625" customWidth="1"/>
+    <col min="8" max="8" width="2.7109375" customWidth="1"/>
+    <col min="9" max="9" width="12.85546875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="2:9" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" s="35" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="40" t="s">
+        <v>21</v>
+      </c>
+      <c r="H3" s="33" t="s">
+        <v>27</v>
+      </c>
+      <c r="I3" s="34"/>
+    </row>
+    <row r="4" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="36"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="41"/>
+      <c r="H4" s="24">
+        <v>1</v>
+      </c>
+      <c r="I4" s="18" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="8">
+        <v>3</v>
+      </c>
+      <c r="C5" s="8">
+        <v>1</v>
+      </c>
+      <c r="D5" s="8">
+        <v>180</v>
+      </c>
+      <c r="E5" s="8">
+        <v>1</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H5" s="25">
+        <v>2</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B6" s="8">
+        <v>4</v>
+      </c>
+      <c r="C6" s="8">
+        <v>2</v>
+      </c>
+      <c r="D6" s="8">
+        <v>82</v>
+      </c>
+      <c r="E6" s="8">
+        <v>3</v>
+      </c>
+      <c r="F6" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H6" s="26">
+        <v>3</v>
+      </c>
+      <c r="I6" s="28" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="8">
+        <v>5</v>
+      </c>
+      <c r="C7" s="8">
+        <v>3</v>
+      </c>
+      <c r="D7" s="8">
+        <v>480</v>
+      </c>
+      <c r="E7" s="8">
+        <v>2</v>
+      </c>
+      <c r="F7" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H7" s="21">
+        <v>4</v>
+      </c>
+      <c r="I7" s="19" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B8" s="8">
+        <v>12</v>
+      </c>
+      <c r="C8" s="8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="8">
+        <v>80</v>
+      </c>
+      <c r="E8" s="8">
+        <v>3</v>
+      </c>
+      <c r="F8" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B9" s="8">
+        <v>13</v>
+      </c>
+      <c r="C9" s="8">
+        <v>2</v>
+      </c>
+      <c r="D9" s="8">
+        <v>350</v>
+      </c>
+      <c r="E9" s="8">
+        <v>3</v>
+      </c>
+      <c r="F9" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B10" s="8">
+        <v>14</v>
+      </c>
+      <c r="C10" s="8">
+        <v>3</v>
+      </c>
+      <c r="D10" s="8">
+        <v>500</v>
+      </c>
+      <c r="E10" s="8">
+        <v>2</v>
+      </c>
+      <c r="F10" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="8">
+        <v>15</v>
+      </c>
+      <c r="C11" s="8">
+        <v>5</v>
+      </c>
+      <c r="D11" s="8">
+        <v>0</v>
+      </c>
+      <c r="E11" s="8">
+        <v>4</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B12" s="8">
+        <v>23</v>
+      </c>
+      <c r="C12" s="8">
+        <v>6</v>
+      </c>
+      <c r="D12" s="8">
+        <v>0</v>
+      </c>
+      <c r="E12" s="8">
+        <v>4</v>
+      </c>
+      <c r="F12" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B13" s="8">
+        <v>24</v>
+      </c>
+      <c r="C13" s="8">
+        <v>2</v>
+      </c>
+      <c r="D13" s="8">
+        <v>220</v>
+      </c>
+      <c r="E13" s="8">
+        <v>3</v>
+      </c>
+      <c r="F13" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="8">
+        <v>32</v>
+      </c>
+      <c r="C14" s="8">
+        <v>5</v>
+      </c>
+      <c r="D14" s="8">
+        <v>0</v>
+      </c>
+      <c r="E14" s="8">
+        <v>4</v>
+      </c>
+      <c r="F14" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B15" s="8">
+        <v>37</v>
+      </c>
+      <c r="C15" s="8">
+        <v>3</v>
+      </c>
+      <c r="D15" s="8">
+        <v>225</v>
+      </c>
+      <c r="E15" s="8">
+        <v>2</v>
+      </c>
+      <c r="F15" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B16" s="8">
+        <v>40</v>
+      </c>
+      <c r="C16" s="8">
+        <v>2</v>
+      </c>
+      <c r="D16" s="8">
+        <v>250</v>
+      </c>
+      <c r="E16" s="8">
+        <v>1</v>
+      </c>
+      <c r="F16" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="8">
+        <v>46</v>
+      </c>
+      <c r="C17" s="8">
+        <v>5</v>
+      </c>
+      <c r="D17" s="8">
+        <v>0</v>
+      </c>
+      <c r="E17" s="8">
+        <v>4</v>
+      </c>
+      <c r="F17" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="8">
+        <v>47</v>
+      </c>
+      <c r="C18" s="8">
+        <v>6</v>
+      </c>
+      <c r="D18" s="8">
+        <v>0</v>
+      </c>
+      <c r="E18" s="8">
+        <v>4</v>
+      </c>
+      <c r="F18" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="8">
+        <v>53</v>
+      </c>
+      <c r="C19" s="8">
+        <v>7</v>
+      </c>
+      <c r="D19" s="8">
+        <v>0</v>
+      </c>
+      <c r="E19" s="8">
+        <v>4</v>
+      </c>
+      <c r="F19" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="8">
+        <v>54</v>
+      </c>
+      <c r="C20" s="8">
+        <v>3</v>
+      </c>
+      <c r="D20" s="8">
+        <v>350</v>
+      </c>
+      <c r="E20" s="8">
+        <v>2</v>
+      </c>
+      <c r="F20" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="C2:C20"/>
+  <mergeCells count="6">
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="D3:D4"/>
+    <mergeCell ref="E3:E4"/>
+    <mergeCell ref="F3:F4"/>
+    <mergeCell ref="H3:I3"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:C13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4770,6 +5127,11 @@
       </c>
     </row>
     <row r="12" spans="2:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="13" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>50</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="C2:C11"/>
   <mergeCells count="2">
@@ -4780,7 +5142,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:G18"/>
   <sheetViews>
@@ -4999,7 +5361,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:D18"/>
   <sheetViews>

</xml_diff>